<commit_message>
# 尝试使用Monster表 todo 读json坏了
</commit_message>
<xml_diff>
--- a/Assets/Other/Excel/MonsterConfig.xlsx
+++ b/Assets/Other/Excel/MonsterConfig.xlsx
@@ -7,9 +7,11 @@
     <workbookView windowWidth="22368" windowHeight="9420"/>
   </bookViews>
   <sheets>
-    <sheet name="#MonsterList" sheetId="1" r:id="rId1"/>
+    <sheet name="#MonsterData" sheetId="1" r:id="rId1"/>
     <sheet name="MonsterRace" sheetId="4" r:id="rId2"/>
-    <sheet name="MonsterTemplate" sheetId="3" r:id="rId3"/>
+    <sheet name="MonsterRaceDetail" sheetId="5" r:id="rId3"/>
+    <sheet name="MonsterJob" sheetId="6" r:id="rId4"/>
+    <sheet name="MonsterTemplate" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -21,7 +23,7 @@
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="G3" authorId="0">
+    <comment ref="H3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="66">
   <si>
     <t>AppType.ClientH |  AppType.ClientM | AppType.Gate | AppType.Map</t>
   </si>
@@ -53,12 +55,15 @@
     <t>Id</t>
   </si>
   <si>
+    <t>种族id</t>
+  </si>
+  <si>
+    <t>种族</t>
+  </si>
+  <si>
     <t>种族1（枚举）</t>
   </si>
   <si>
-    <t>种族</t>
-  </si>
-  <si>
     <t>名字</t>
   </si>
   <si>
@@ -95,12 +100,15 @@
     <t>特质修正（几个池子，根据权重随机）</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>RaceName</t>
+  </si>
+  <si>
     <t>CreatureRaceType</t>
   </si>
   <si>
-    <t>RaceName</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -131,12 +139,12 @@
     <t>int</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
     <t>enum_CreatureRaceType</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>int[]</t>
   </si>
   <si>
@@ -155,42 +163,42 @@
     <t>Beast</t>
   </si>
   <si>
+    <t>幼犬</t>
+  </si>
+  <si>
+    <t>1,70,2,30</t>
+  </si>
+  <si>
+    <t>Power_Set_2</t>
+  </si>
+  <si>
+    <t>幼崽</t>
+  </si>
+  <si>
+    <t>无</t>
+  </si>
+  <si>
+    <t>离群野犬</t>
+  </si>
+  <si>
+    <t>成熟</t>
+  </si>
+  <si>
+    <t>流浪犬</t>
+  </si>
+  <si>
+    <t>野犬猎手</t>
+  </si>
+  <si>
+    <t>猎手</t>
+  </si>
+  <si>
+    <t>野犬王者</t>
+  </si>
+  <si>
     <t>狂犬</t>
   </si>
   <si>
-    <t>幼犬</t>
-  </si>
-  <si>
-    <t>1,70,2,30</t>
-  </si>
-  <si>
-    <t>Power_Set_2</t>
-  </si>
-  <si>
-    <t>幼崽</t>
-  </si>
-  <si>
-    <t>无</t>
-  </si>
-  <si>
-    <t>离群野犬</t>
-  </si>
-  <si>
-    <t>成熟</t>
-  </si>
-  <si>
-    <t>流浪犬</t>
-  </si>
-  <si>
-    <t>野犬猎手</t>
-  </si>
-  <si>
-    <t>猎手</t>
-  </si>
-  <si>
-    <t>野犬王者</t>
-  </si>
-  <si>
     <t>母体</t>
   </si>
   <si>
@@ -207,6 +215,15 @@
   </si>
   <si>
     <t>种族名</t>
+  </si>
+  <si>
+    <t>可出现的职业</t>
+  </si>
+  <si>
+    <t>野兽</t>
+  </si>
+  <si>
+    <t>浮游</t>
   </si>
   <si>
     <t>种族等级</t>
@@ -229,10 +246,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -270,16 +287,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -292,8 +301,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,14 +329,6 @@
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -371,20 +380,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -400,8 +402,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,7 +444,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,7 +462,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,7 +480,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,121 +594,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,19 +624,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,21 +635,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -647,6 +649,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -671,15 +682,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -718,6 +720,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -726,10 +743,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -738,16 +755,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -759,10 +776,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -774,101 +794,98 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -879,6 +896,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
@@ -1229,10 +1249,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1240,24 +1260,25 @@
     <col min="1" max="1" width="13.7777777777778" customWidth="1"/>
     <col min="2" max="2" width="16.1111111111111" customWidth="1"/>
     <col min="3" max="3" width="4.66666666666667" customWidth="1"/>
-    <col min="4" max="4" width="31.8888888888889" customWidth="1"/>
+    <col min="4" max="4" width="8.22222222222222" customWidth="1"/>
     <col min="5" max="5" width="14.2222222222222" customWidth="1"/>
-    <col min="6" max="6" width="15.8888888888889" customWidth="1"/>
-    <col min="7" max="7" width="7.55555555555556" customWidth="1"/>
-    <col min="8" max="9" width="15.8888888888889" customWidth="1"/>
-    <col min="10" max="10" width="32.1111111111111" customWidth="1"/>
-    <col min="11" max="11" width="15.8888888888889" customWidth="1"/>
-    <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="33.5555555555556" customWidth="1"/>
-    <col min="14" max="14" width="21" customWidth="1"/>
-    <col min="15" max="15" width="17.1111111111111" customWidth="1"/>
-    <col min="16" max="16" width="15.8888888888889" customWidth="1"/>
-    <col min="17" max="17" width="17.6666666666667" customWidth="1"/>
-    <col min="18" max="18" width="32.1111111111111" customWidth="1"/>
-    <col min="19" max="19" width="43.1111111111111" customWidth="1"/>
+    <col min="6" max="6" width="31.8888888888889" customWidth="1"/>
+    <col min="7" max="7" width="15.8888888888889" customWidth="1"/>
+    <col min="8" max="8" width="7.55555555555556" customWidth="1"/>
+    <col min="9" max="10" width="15.8888888888889" customWidth="1"/>
+    <col min="11" max="11" width="32.1111111111111" customWidth="1"/>
+    <col min="12" max="12" width="15.8888888888889" customWidth="1"/>
+    <col min="13" max="13" width="8" customWidth="1"/>
+    <col min="14" max="14" width="33.5555555555556" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
+    <col min="16" max="16" width="17.1111111111111" customWidth="1"/>
+    <col min="17" max="17" width="15.8888888888889" customWidth="1"/>
+    <col min="18" max="18" width="17.6666666666667" customWidth="1"/>
+    <col min="19" max="19" width="32.1111111111111" customWidth="1"/>
+    <col min="20" max="20" width="43.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.4" spans="1:20">
+    <row r="1" ht="17.4" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1280,8 +1301,9 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
-    </row>
-    <row r="2" ht="17.4" spans="1:20">
+      <c r="U1" s="1"/>
+    </row>
+    <row r="2" ht="17.4" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1306,8 +1328,9 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
-    </row>
-    <row r="3" ht="17.4" spans="1:20">
+      <c r="U2" s="1"/>
+    </row>
+    <row r="3" ht="17.4" spans="1:21">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
@@ -1337,10 +1360,10 @@
       <c r="K3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1353,928 +1376,983 @@
         <v>16</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T3" s="1"/>
-    </row>
-    <row r="4" ht="17.4" spans="1:20">
+        <v>11</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" ht="17.4" spans="1:21">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="L4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="N4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="2"/>
       <c r="R4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" s="1"/>
-    </row>
-    <row r="5" ht="17.4" spans="1:20">
+        <v>27</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" ht="17.4" spans="1:21">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" ht="17.4" spans="1:20">
+      <c r="T5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" ht="17.4" spans="1:21">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>38</v>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="str">
+        <f>VLOOKUP(D6,MonsterRace!$C:$D,2,)</f>
+        <v>野兽</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="3">
         <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="3">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3">
         <v>1</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R6" s="3"/>
+      <c r="R6" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-    </row>
-    <row r="7" ht="17.4" spans="1:20">
+      <c r="U6" s="3"/>
+    </row>
+    <row r="7" ht="17.4" spans="1:21">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>38</v>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="str">
+        <f>VLOOKUP(D7,MonsterRace!$C:$D,2,)</f>
+        <v>野兽</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="3">
+        <v>39</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="3">
         <v>4</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3">
+      <c r="M7" s="3"/>
+      <c r="N7" s="3">
         <v>1</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="3">
         <v>0.5</v>
       </c>
-      <c r="Q7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R7" s="3"/>
+      <c r="R7" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-    </row>
-    <row r="8" ht="17.4" spans="1:20">
+      <c r="U7" s="3"/>
+    </row>
+    <row r="8" ht="17.4" spans="1:21">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
         <v>3</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>38</v>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="str">
+        <f>VLOOKUP(D8,MonsterRace!$C:$D,2,)</f>
+        <v>野兽</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="3">
+        <v>39</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="3">
         <v>5</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="3">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3">
         <v>1</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="O8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P8" s="3">
+        <v>46</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q8" s="3">
         <v>0.6</v>
       </c>
-      <c r="Q8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R8" s="3"/>
+      <c r="R8" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
-    </row>
-    <row r="9" ht="17.4" spans="1:20">
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" ht="17.4" spans="1:21">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>38</v>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="str">
+        <f>VLOOKUP(D9,MonsterRace!$C:$D,2,)</f>
+        <v>野兽</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="3">
+        <v>39</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="3">
         <v>7</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="M9" s="3"/>
       <c r="N9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="P9" s="3">
+        <v>51</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="3">
         <v>1</v>
       </c>
-      <c r="Q9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R9" s="3"/>
+      <c r="R9" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-    </row>
-    <row r="10" ht="17.4" spans="1:20">
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" ht="17.4" spans="1:21">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="3">
         <v>5</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="4">
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="str">
+        <f>VLOOKUP(D10,MonsterRace!$C:$D,2,)</f>
+        <v>野兽</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="4">
         <v>6</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="K10" s="3"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
       <c r="N10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="P10" s="3">
+        <v>54</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q10" s="3">
         <v>0.7</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R10" s="3"/>
-      <c r="S10" s="1"/>
+      <c r="R10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" s="3"/>
       <c r="T10" s="1"/>
-    </row>
-    <row r="11" ht="17.4" spans="1:20">
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" ht="17.4" spans="1:21">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="1"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="1"/>
       <c r="N11" s="4"/>
-      <c r="P11" s="1"/>
+      <c r="O11" s="4"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
-    </row>
-    <row r="12" ht="17.4" spans="1:20">
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" ht="17.4" spans="1:21">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="1"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="1"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="3"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="1"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="1"/>
+      <c r="S12" s="3"/>
       <c r="T12" s="1"/>
-    </row>
-    <row r="13" ht="17.4" spans="1:20">
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" ht="17.4" spans="1:21">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="1"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="1"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="3"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="1"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="1"/>
+      <c r="S13" s="3"/>
       <c r="T13" s="1"/>
-    </row>
-    <row r="14" ht="17.4" spans="1:20">
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" ht="17.4" spans="1:21">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="1"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="4"/>
+      <c r="M14" s="1"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="3"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="1"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="1"/>
+      <c r="S14" s="3"/>
       <c r="T14" s="1"/>
-    </row>
-    <row r="15" ht="17.4" spans="1:20">
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" ht="17.4" spans="1:21">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="1"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="4"/>
+      <c r="M15" s="1"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="3"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="1"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="1"/>
+      <c r="S15" s="3"/>
       <c r="T15" s="1"/>
-    </row>
-    <row r="16" ht="17.4" spans="1:20">
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" ht="17.4" spans="1:21">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="1"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="4"/>
+      <c r="M16" s="1"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="3"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="1"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="1"/>
+      <c r="S16" s="3"/>
       <c r="T16" s="1"/>
-    </row>
-    <row r="17" ht="17.4" spans="1:20">
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" ht="17.4" spans="1:21">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="1"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="4"/>
+      <c r="M17" s="1"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="3"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="1"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="1"/>
+      <c r="S17" s="3"/>
       <c r="T17" s="1"/>
-    </row>
-    <row r="18" ht="17.4" spans="1:20">
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" ht="17.4" spans="1:21">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="1"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="4"/>
+      <c r="M18" s="1"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="1"/>
+      <c r="P18" s="4"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
-    </row>
-    <row r="19" ht="17.4" spans="1:20">
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" ht="17.4" spans="1:21">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="1"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="4"/>
+      <c r="M19" s="1"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="1"/>
+      <c r="P19" s="4"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
-    </row>
-    <row r="20" ht="17.4" spans="1:20">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" ht="17.4" spans="1:21">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="1"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="1"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="1"/>
+      <c r="P20" s="4"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
-    </row>
-    <row r="21" ht="17.4" spans="1:20">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" ht="17.4" spans="1:21">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="1"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="4"/>
+      <c r="M21" s="1"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="1"/>
+      <c r="P21" s="4"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
-    </row>
-    <row r="22" ht="17.4" spans="1:20">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" ht="17.4" spans="1:21">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="1"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="4"/>
+      <c r="M22" s="1"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="1"/>
+      <c r="P22" s="4"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
-    </row>
-    <row r="23" ht="17.4" spans="1:20">
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" ht="17.4" spans="1:21">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="1"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="4"/>
+      <c r="M23" s="1"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
-      <c r="P23" s="1"/>
+      <c r="P23" s="4"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
-    </row>
-    <row r="24" ht="17.4" spans="1:20">
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" ht="17.4" spans="1:21">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="1"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="4"/>
+      <c r="M24" s="1"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
-      <c r="P24" s="1"/>
+      <c r="P24" s="4"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
-    </row>
-    <row r="25" ht="17.4" spans="1:20">
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" ht="17.4" spans="1:21">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="1"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="4"/>
+      <c r="M25" s="1"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
-      <c r="P25" s="1"/>
+      <c r="P25" s="4"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
-    </row>
-    <row r="26" ht="17.4" spans="1:20">
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" ht="17.4" spans="1:21">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="1"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="4"/>
+      <c r="M26" s="1"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
-      <c r="P26" s="1"/>
+      <c r="P26" s="4"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-    </row>
-    <row r="27" ht="17.4" spans="1:20">
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" ht="17.4" spans="1:21">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="1"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="4"/>
+      <c r="M27" s="1"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
-      <c r="P27" s="1"/>
+      <c r="P27" s="4"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
-    </row>
-    <row r="28" ht="17.4" spans="1:20">
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" ht="17.4" spans="1:21">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="1"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="4"/>
+      <c r="M28" s="1"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28" s="1"/>
+      <c r="P28" s="4"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
-    </row>
-    <row r="29" ht="17.4" spans="1:20">
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" ht="17.4" spans="1:21">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="1"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="4"/>
+      <c r="M29" s="1"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-      <c r="P29" s="1"/>
+      <c r="P29" s="4"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
-    </row>
-    <row r="30" ht="17.4" spans="1:20">
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" ht="17.4" spans="1:21">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="1"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="4"/>
+      <c r="M30" s="1"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
-      <c r="P30" s="1"/>
+      <c r="P30" s="4"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
-    </row>
-    <row r="31" ht="17.4" spans="1:20">
+      <c r="U30" s="1"/>
+    </row>
+    <row r="31" ht="17.4" spans="1:21">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="1"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="4"/>
+      <c r="M31" s="1"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
-      <c r="P31" s="1"/>
+      <c r="P31" s="4"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
-    </row>
-    <row r="32" ht="17.4" spans="1:20">
+      <c r="U31" s="1"/>
+    </row>
+    <row r="32" ht="17.4" spans="1:21">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="1"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="4"/>
+      <c r="M32" s="1"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
-      <c r="P32" s="1"/>
+      <c r="P32" s="4"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
-    </row>
-    <row r="33" ht="17.4" spans="1:20">
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" ht="17.4" spans="1:21">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="1"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="4"/>
+      <c r="M33" s="1"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="1"/>
+      <c r="P33" s="4"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
-    </row>
-    <row r="34" ht="17.4" spans="1:20">
+      <c r="U33" s="1"/>
+    </row>
+    <row r="34" ht="17.4" spans="1:21">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="1"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-      <c r="M34" s="4"/>
+      <c r="M34" s="1"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-      <c r="P34" s="1"/>
+      <c r="P34" s="4"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
-    </row>
-    <row r="35" ht="17.4" spans="1:20">
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" ht="17.4" spans="1:21">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="1"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="4"/>
+      <c r="M35" s="1"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-      <c r="P35" s="1"/>
+      <c r="P35" s="4"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
-    </row>
-    <row r="36" ht="17.4" spans="1:20">
+      <c r="U35" s="1"/>
+    </row>
+    <row r="36" ht="17.4" spans="1:21">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="1"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="4"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="4"/>
+      <c r="M36" s="1"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-      <c r="P36" s="1"/>
+      <c r="P36" s="4"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
-    </row>
-    <row r="37" ht="17.4" spans="1:20">
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" ht="17.4" spans="1:21">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="4"/>
@@ -2293,10 +2371,11 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
-      <c r="S37" s="1"/>
+      <c r="S37" s="4"/>
       <c r="T37" s="1"/>
-    </row>
-    <row r="38" ht="17.4" spans="1:20">
+      <c r="U37" s="1"/>
+    </row>
+    <row r="38" ht="17.4" spans="1:21">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2317,8 +2396,9 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
-    </row>
-    <row r="39" ht="17.4" spans="1:20">
+      <c r="U38" s="1"/>
+    </row>
+    <row r="39" ht="17.4" spans="1:21">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2339,8 +2419,9 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
-    </row>
-    <row r="40" ht="17.4" spans="1:20">
+      <c r="U39" s="1"/>
+    </row>
+    <row r="40" ht="17.4" spans="1:21">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2361,8 +2442,9 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
-    </row>
-    <row r="41" ht="17.4" spans="1:20">
+      <c r="U40" s="1"/>
+    </row>
+    <row r="41" ht="17.4" spans="1:21">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2383,6 +2465,7 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2395,10 +2478,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2407,18 +2490,501 @@
     <col min="2" max="2" width="16.2222222222222" customWidth="1"/>
     <col min="3" max="3" width="4.66666666666667" customWidth="1"/>
     <col min="4" max="4" width="8.33333333333333" customWidth="1"/>
-    <col min="5" max="5" width="31.8888888888889" customWidth="1"/>
-    <col min="6" max="6" width="33.5555555555556" customWidth="1"/>
-    <col min="7" max="7" width="10.6666666666667" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="17.1111111111111" customWidth="1"/>
-    <col min="10" max="11" width="15.8888888888889" customWidth="1"/>
-    <col min="12" max="12" width="17.6666666666667" customWidth="1"/>
-    <col min="13" max="13" width="32.1111111111111" customWidth="1"/>
-    <col min="14" max="14" width="43.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="17.1111111111111" customWidth="1"/>
+    <col min="6" max="6" width="17.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="32.1111111111111" customWidth="1"/>
+    <col min="8" max="8" width="43.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.4" spans="1:15">
+    <row r="1" ht="17.4" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" ht="17.4" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" ht="17.4" spans="1:9">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" ht="17.4" spans="1:9">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" ht="17.4" spans="1:9">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" ht="17.4" spans="1:9">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" ht="17.4" spans="1:9">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" ht="17.4" spans="1:9">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" ht="17.4" spans="1:9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" ht="17.4" spans="1:9">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" ht="17.4" spans="1:9">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" ht="17.4" spans="1:9">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" ht="17.4" spans="1:9">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" ht="17.4" spans="1:9">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" ht="17.4" spans="1:9">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" ht="17.4" spans="1:9">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" ht="17.4" spans="1:9">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" ht="17.4" spans="1:9">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" ht="17.4" spans="1:9">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" ht="17.4" spans="1:9">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" ht="17.4" spans="1:9">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" ht="17.4" spans="1:9">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" ht="17.4" spans="1:9">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" ht="17.4" spans="1:9">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" ht="17.4" spans="1:9">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" ht="17.4" spans="1:9">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" ht="17.4" spans="1:9">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" ht="17.4" spans="1:9">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" ht="17.4" spans="1:9">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" ht="17.4" spans="1:9">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" ht="17.4" spans="1:9">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" ht="17.4" spans="1:9">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" ht="17.4" spans="1:9">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" ht="17.4" spans="1:9">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" ht="17.4" spans="1:9">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" ht="17.4" spans="1:9">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" ht="17.4" spans="1:9">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="7"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16.2222222222222" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="17.4" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2435,14 +3001,13 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" ht="17.4" spans="1:15">
+    </row>
+    <row r="2" ht="17.4" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2456,188 +3021,203 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" ht="17.4" spans="1:15">
+    </row>
+    <row r="3" ht="17.4" spans="1:14">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" ht="17.4" spans="1:15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" ht="17.4" spans="1:14">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" ht="17.4" spans="1:15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" ht="17.4" spans="1:14">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="N5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" ht="17.4" spans="1:15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" ht="17.4" spans="1:14">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G6" s="3">
         <v>8</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K6" s="3">
         <v>0.2</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" ht="17.4" spans="1:15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" ht="17.4" spans="1:15">
+    </row>
+    <row r="7" ht="17.4" spans="1:14">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="3">
+        <v>8</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" ht="17.4" spans="1:14">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -2648,509 +3228,30 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" ht="17.4" spans="1:15">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" ht="17.4" spans="1:15">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" ht="17.4" spans="1:15">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" ht="17.4" spans="1:15">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" ht="17.4" spans="1:15">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" ht="17.4" spans="1:15">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" ht="17.4" spans="1:15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" ht="17.4" spans="1:15">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" ht="17.4" spans="1:15">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" ht="17.4" spans="1:15">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" ht="17.4" spans="1:15">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" ht="17.4" spans="1:15">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" ht="17.4" spans="1:15">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" ht="17.4" spans="1:15">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" ht="17.4" spans="1:15">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" ht="17.4" spans="1:15">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" ht="17.4" spans="1:15">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" ht="17.4" spans="1:15">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" ht="17.4" spans="1:15">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-    </row>
-    <row r="28" ht="17.4" spans="1:15">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-    </row>
-    <row r="29" ht="17.4" spans="1:15">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-    </row>
-    <row r="30" ht="17.4" spans="1:15">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-    </row>
-    <row r="31" ht="17.4" spans="1:15">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-    </row>
-    <row r="32" ht="17.4" spans="1:15">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-    </row>
-    <row r="33" ht="17.4" spans="1:15">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-    </row>
-    <row r="34" ht="17.4" spans="1:15">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-    </row>
-    <row r="35" ht="17.4" spans="1:15">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-    </row>
-    <row r="36" ht="17.4" spans="1:15">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-    </row>
-    <row r="37" ht="17.4" spans="1:15">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:L38"/>
@@ -3213,26 +3314,26 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L3" s="1"/>
     </row>
@@ -3243,24 +3344,24 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L4" s="1"/>
     </row>
@@ -3268,29 +3369,29 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L5" s="1"/>
     </row>
@@ -3301,20 +3402,20 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H6" s="3">
         <v>0.2</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -3327,20 +3428,20 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H7" s="3">
         <v>0.5</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -3353,20 +3454,20 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="H8" s="3">
         <v>0.6</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>

</xml_diff>